<commit_message>
update to add addDataBase function
</commit_message>
<xml_diff>
--- a/miniproject/template/Lectures/Lecture 1.xlsx
+++ b/miniproject/template/Lectures/Lecture 1.xlsx
@@ -40,7 +40,7 @@
     <t>Meaning</t>
   </si>
   <si>
-    <t>Meaning（中文）</t>
+    <t>Translation</t>
   </si>
   <si>
     <t>level_2</t>
@@ -1028,11 +1028,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1076,12 +1076,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -1089,9 +1083,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1104,28 +1120,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1144,21 +1146,6 @@
       <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1186,23 +1173,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1223,6 +1210,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -1231,9 +1225,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1264,31 +1258,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1306,13 +1294,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1324,7 +1306,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1348,19 +1348,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1372,43 +1390,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1426,25 +1408,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1491,17 +1485,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1521,6 +1506,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1532,15 +1535,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1560,6 +1554,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1574,113 +1579,102 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1689,49 +1683,49 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1778,13 +1772,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2108,8 +2102,8 @@
   <sheetPr/>
   <dimension ref="A1:AG187"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="X1" sqref="V1:X1"/>
+    <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66071428571429" defaultRowHeight="11.6"/>

</xml_diff>